<commit_message>
p and sample size
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halsayxi\Desktop\thuirlab\组会\20250910\final_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3737E2E9-9811-4FC2-B84A-7646C3978DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6133F8-B576-4307-B78A-E395CD067F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{1A10E913-6A1E-4376-880A-22B7F29311FC}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>Variable</t>
   </si>
@@ -349,10 +349,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>p_value</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>llm_ATE</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -372,14 +368,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>***  p &lt; 0.01  
-**   0.01 &lt;= p &lt; 0.05  
-*    0.05 &lt;= p &lt; 0.1  
-n.s. p &gt;= 0.1  
-numeric value = exact p-value (e.g., p = 0.023)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Average Treatment Effect, representing the average difference in daily usage per person between the treated group and the control group (LLM)</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -393,6 +381,23 @@
   </si>
   <si>
     <t>Robust Standard Error of the ATE, measuring the estimation precision of the treatment effect (human)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1 = Significant (p &lt; 0.1)  
+0 = Not significant (p &gt;= 0.1) </t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>significance_binary</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sample_size_replication</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample size in the replication experiment</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1348,10 +1353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2CCBDC-6639-474A-A78B-1A7B5002B89B}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1493,7 +1498,7 @@
         <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1520,255 +1525,263 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="56" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="56" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>39</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>95</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="28" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="84" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" t="s">
-        <v>101</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>58</v>
-      </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>100</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>87</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="112" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" ht="112" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>81</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="70" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="48" spans="1:3" ht="70" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>82</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>89</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>